<commit_message>
Eigengene mappings, cell type mapping function
</commit_message>
<xml_diff>
--- a/inst/extdata/cell_type_mapping.xlsx
+++ b/inst/extdata/cell_type_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/massoudmaher/Documents/Code/immunedeconv/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080301E4-E49B-0949-985F-458DC85F8567}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F32C02-174C-5642-B35F-CFCA39BAADE9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="460" windowWidth="27100" windowHeight="17080" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1328,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK66"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3018,7 +3018,7 @@
   <dimension ref="A1:F243"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D184" sqref="D184"/>
+      <selection activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>